<commit_message>
refactor: ajust assessment doc
</commit_message>
<xml_diff>
--- a/trabalho-final/docs/assessment/assessment.xlsx
+++ b/trabalho-final/docs/assessment/assessment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo" sheetId="1" state="visible" r:id="rId2"/>
@@ -404,7 +404,7 @@
     <t xml:space="preserve">ParentProductCategoryID</t>
   </si>
   <si>
-    <t xml:space="preserve">Foreign Key recursiva dentro da categoria do produto</t>
+    <t xml:space="preserve">Foreign Key recursiva dentro da categoria do produto. Identifica qual é a categoria raiz</t>
   </si>
   <si>
     <t xml:space="preserve">Nome da categoria do produto</t>
@@ -715,9 +715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>93600</xdr:colOff>
+      <xdr:colOff>93240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -731,7 +731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="31680" y="0"/>
-          <a:ext cx="8415720" cy="6515640"/>
+          <a:ext cx="8415360" cy="6515280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -754,7 +754,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -778,7 +778,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="1" sqref="B13 H7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -945,7 +945,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="B13 B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1222,7 +1222,7 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1742,7 +1742,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B13 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2006,7 +2006,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2411,8 +2411,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="B13 D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2424,7 +2424,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="70.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2579,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2726,7 +2726,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="1" sqref="B13 H7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2886,7 +2886,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="1" sqref="B13 H6"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3052,7 +3052,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="B13 H17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>